<commit_message>
Scroll bars + more google drive
Scroll bars for UI
Google drive now work with all word docs (instruction sheets) and spreadsheets (formulation templates and ingredients df)
</commit_message>
<xml_diff>
--- a/Restored To Eden/Outputs/Sheets/monni hardstone Jul-11-2020/oil cleanser.xlsx
+++ b/Restored To Eden/Outputs/Sheets/monni hardstone Jul-11-2020/oil cleanser.xlsx
@@ -85,64 +85,64 @@
     <t>Additional Benefits</t>
   </si>
   <si>
+    <t>peeling</t>
+  </si>
+  <si>
+    <t>peeling and dehydrated (due to use of products to control oil)</t>
+  </si>
+  <si>
+    <t>rough on some portions of the skin</t>
+  </si>
+  <si>
+    <t>clogged pores/cell accumulation</t>
+  </si>
+  <si>
+    <t>pre-disposed to acne</t>
+  </si>
+  <si>
+    <t>excessive oil in some areas (possibly int he t-zone)</t>
+  </si>
+  <si>
     <t>scaling</t>
   </si>
   <si>
+    <t>dry/rough skin in feeling and/or appearance/rough skin in feeling and/or appearance and/or flaky on some portions of skin</t>
+  </si>
+  <si>
+    <t>inflamed and/or irritated</t>
+  </si>
+  <si>
+    <t>dry/rough skin in feeling and/or appearance</t>
+  </si>
+  <si>
+    <t>oily (overproduction of sebum)</t>
+  </si>
+  <si>
     <t>dry</t>
   </si>
   <si>
-    <t>clogged pores/cell accumulation</t>
-  </si>
-  <si>
     <t>tewl</t>
   </si>
   <si>
-    <t>oily (overproduction of sebum)</t>
+    <t>flaking</t>
+  </si>
+  <si>
+    <t>eczema</t>
+  </si>
+  <si>
+    <t>enlarged pores</t>
   </si>
   <si>
     <t>itchy</t>
   </si>
   <si>
-    <t>enlarged pores</t>
+    <t>sensitive</t>
+  </si>
+  <si>
+    <t>itching and/or redness</t>
   </si>
   <si>
     <t>chapped</t>
-  </si>
-  <si>
-    <t>dry/rough skin in feeling and/or appearance/rough skin in feeling and/or appearance and/or flaky on some portions of skin</t>
-  </si>
-  <si>
-    <t>rough on some portions of the skin</t>
-  </si>
-  <si>
-    <t>flaking</t>
-  </si>
-  <si>
-    <t>dry/rough skin in feeling and/or appearance</t>
-  </si>
-  <si>
-    <t>eczema</t>
-  </si>
-  <si>
-    <t>pre-disposed to acne</t>
-  </si>
-  <si>
-    <t>inflamed and/or irritated</t>
-  </si>
-  <si>
-    <t>sensitive</t>
-  </si>
-  <si>
-    <t>itching and/or redness</t>
-  </si>
-  <si>
-    <t>peeling and dehydrated (due to use of products to control oil)</t>
-  </si>
-  <si>
-    <t>peeling</t>
-  </si>
-  <si>
-    <t>excessive oil in some areas (possibly int he t-zone)</t>
   </si>
 </sst>
 </file>

</xml_diff>